<commit_message>
Fix for multiple result
</commit_message>
<xml_diff>
--- a/files/TRAVIS COUNTY.xlsx
+++ b/files/TRAVIS COUNTY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriezennmagbanua/Projects/Personal/Tool/address-scrape-tool/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054F7911-2898-6B4D-B238-1DA75309A5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783E864-4EE2-CF45-AF78-283E6FBD56EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>4305 Leslie Ave</t>
   </si>
   <si>
-    <t>4709 Gonzales St #A</t>
-  </si>
-  <si>
     <t>17808 Maritime Point Dr 202</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>1301 W 29 St</t>
+  </si>
+  <si>
+    <t>4709 Gonzales St</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -612,7 +612,7 @@
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>24</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>24</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>24</v>

</xml_diff>